<commit_message>
Reorganizing files and updates to README for grading
</commit_message>
<xml_diff>
--- a/Hyperparameter tracker.xlsx
+++ b/Hyperparameter tracker.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Folders\Education\UCI\23 Fall\CS 175\MsPacman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2992EB13-F868-4A22-92D9-2B8457212262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBCF4AE-CA52-43EB-A2B7-4D35EA7746E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9255" yWindow="1965" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3285" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy" sheetId="1" r:id="rId1"/>
-    <sheet name="Optuna Study" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Std</t>
   </si>
@@ -140,6 +150,57 @@
   </si>
   <si>
     <t>Policy file name</t>
+  </si>
+  <si>
+    <t>MsPacManPG_optimized.pt</t>
+  </si>
+  <si>
+    <t>hyperparameters = {
+    'gamma': 0.9999819193245816, 
+    'n_layers': 1, 
+    'h_size': 175, 
+    'dropout': 0.44984866197635065, 
+    'lr': 6.166629462708628e-05, 
+    'longevity_exponential': 1.006491852944776, 
+    'step_penalty_multiplier': 1.0386448544834312, 
+    'dot_extra_reward': 13, 
+    'energy_pill_extra_reward': 12,
+    "ghost_reward": 0,
+    "optimizer": "SGD",
+    "policy_file_name": "MsPacManPG_optimized.pt",
+    "n_training_episodes": 10000,
+#     "n_evaluation_episodes": 10,
+    "max_t": 50000,
+    "env_id": "ALE/MsPacman-ram-v5",
+    "s_size": 128,
+    "a_size": 5,
+}</t>
+  </si>
+  <si>
+    <t>- MsPacMan_replay_3_best.mp4
+- MsPacMan_replay_3_worst.mp4</t>
+  </si>
+  <si>
+    <t>hyperparameters_1 = {
+    "h_size": 32,
+    "n_training_episodes": 10000,
+    "n_evaluation_episodes": 10,
+    "max_t": 5000,
+    "gamma": 0.99,
+    "lr": 1e-4,
+    "env_id": env_id,
+    "state_space": 128,
+    "action_space": 5,
+}</t>
+  </si>
+  <si>
+    <t>MsPacMan_beforeOptimizing_replay.mp4</t>
+  </si>
+  <si>
+    <t>Final trained agent with improved policy network, rewards, and hyperparameters</t>
+  </si>
+  <si>
+    <t>Trained agent before making improvements to policy network, rewards, and hyperparameters</t>
   </si>
 </sst>
 </file>
@@ -177,7 +238,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,92 +563,109 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
       <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>943</v>
-      </c>
-      <c r="D2">
-        <v>847.18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>10000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
       <c r="B3">
         <v>100</v>
       </c>
       <c r="C3">
-        <v>864</v>
+        <v>943</v>
       </c>
       <c r="D3">
-        <v>566.71</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>847.18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4">
+        <v>864</v>
+      </c>
+      <c r="D4">
+        <v>566.71</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
         <v>712</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>447.83</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>435</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>206.94</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B309D6-12CF-4568-B05A-A035ACCF2373}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>